<commit_message>
Finalise Technical Manual and Agent Manual
</commit_message>
<xml_diff>
--- a/emma/documentation/Use Cases.xlsx
+++ b/emma/documentation/Use Cases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Event</t>
   </si>
@@ -57,33 +57,15 @@
     <t>Ext/St/Temp</t>
   </si>
   <si>
-    <t>(Triggered from Use Case 1)</t>
-  </si>
-  <si>
     <t>1. Send query</t>
   </si>
   <si>
-    <t>3. Update user details</t>
-  </si>
-  <si>
     <t>2. Send user details</t>
   </si>
   <si>
-    <t>4. Look up answer</t>
-  </si>
-  <si>
-    <t>5. Send response</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
-    <t>(Triggered from Use Case 2)</t>
-  </si>
-  <si>
-    <t>(Triggered from Use Case 4)</t>
-  </si>
-  <si>
     <t>QueryID, UserID, Time, Location, Content</t>
   </si>
   <si>
@@ -105,12 +87,6 @@
     <t>User details sent confirmation</t>
   </si>
   <si>
-    <t>User details</t>
-  </si>
-  <si>
-    <t>Query response text</t>
-  </si>
-  <si>
     <t>Answer to query found</t>
   </si>
   <si>
@@ -150,13 +126,55 @@
     <t>CRUD Analysis</t>
   </si>
   <si>
-    <t>Query Content, Time, Location, Audio, Image</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>Agent has no users to assign to themselves</t>
+  </si>
+  <si>
+    <t>3. Assign user</t>
+  </si>
+  <si>
+    <t>(Triggered from Use Case 1 or 2)</t>
+  </si>
+  <si>
+    <t>Agent sees unassigned user in open queue</t>
+  </si>
+  <si>
+    <t>(Triggered from Use Case 3)</t>
+  </si>
+  <si>
+    <t>4. Update user details</t>
+  </si>
+  <si>
+    <t>5. Look up answer</t>
+  </si>
+  <si>
+    <t>6. Send response</t>
+  </si>
+  <si>
+    <t>7. Request user release</t>
+  </si>
+  <si>
+    <t>(Triggered from Use Case 5)</t>
+  </si>
+  <si>
+    <t>UserID, AssignedTo, Status</t>
+  </si>
+  <si>
+    <t>UserID, Query content</t>
+  </si>
+  <si>
+    <t>Query content, Time, Location, Audio, Image</t>
+  </si>
+  <si>
+    <t>AgentID</t>
+  </si>
+  <si>
+    <t>Answer</t>
   </si>
 </sst>
 </file>
@@ -257,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,6 +319,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -594,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,15 +633,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -647,122 +668,142 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2"/>
+      <c r="C5" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="C8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
@@ -778,9 +819,27 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -809,10 +868,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="18"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
@@ -821,10 +880,10 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
-      <c r="B2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="20"/>
       <c r="D2" s="14"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -832,13 +891,13 @@
     </row>
     <row r="3" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="9"/>
@@ -847,13 +906,13 @@
     </row>
     <row r="4" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="9"/>
@@ -862,13 +921,13 @@
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="9"/>
@@ -877,10 +936,10 @@
     </row>
     <row r="6" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="10"/>
@@ -890,13 +949,13 @@
     </row>
     <row r="7" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="9"/>
@@ -905,11 +964,11 @@
     </row>
     <row r="8" spans="1:8" s="8" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="9"/>

</xml_diff>